<commit_message>
ver 0.7.3 correct print graph
</commit_message>
<xml_diff>
--- a/smo/SMO_result.xlsx
+++ b/smo/SMO_result.xlsx
@@ -458,10 +458,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>143535</v>
+        <v>169702.5</v>
       </c>
       <c r="D2" t="n">
-        <v>377.5</v>
+        <v>449.5</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>60667.5</v>
+        <v>89715</v>
       </c>
       <c r="D3" t="n">
-        <v>207.5</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4">
@@ -486,10 +486,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>46485</v>
+        <v>57915</v>
       </c>
       <c r="D4" t="n">
-        <v>205.25</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +500,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>68302.5</v>
+        <v>69637.5</v>
       </c>
       <c r="D5" t="n">
-        <v>205.25</v>
+        <v>210.75</v>
       </c>
     </row>
     <row r="6">
@@ -514,10 +514,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>92460</v>
+        <v>91552.5</v>
       </c>
       <c r="D6" t="n">
-        <v>205.25</v>
+        <v>210.75</v>
       </c>
     </row>
     <row r="7">
@@ -528,10 +528,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>117090</v>
+        <v>115605</v>
       </c>
       <c r="D7" t="n">
-        <v>205.25</v>
+        <v>210.25</v>
       </c>
     </row>
     <row r="8">
@@ -542,10 +542,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>141720</v>
+        <v>140535</v>
       </c>
       <c r="D8" t="n">
-        <v>205.25</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9">
@@ -556,10 +556,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>166350</v>
+        <v>165600</v>
       </c>
       <c r="D9" t="n">
-        <v>205.25</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10">
@@ -570,10 +570,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>190980</v>
+        <v>191317.5</v>
       </c>
       <c r="D10" t="n">
-        <v>205.25</v>
+        <v>210.25</v>
       </c>
     </row>
     <row r="11">
@@ -584,10 +584,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>215610</v>
+        <v>216337.5</v>
       </c>
       <c r="D11" t="n">
-        <v>205.25</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ver 0.7.4 update graph
</commit_message>
<xml_diff>
--- a/smo/SMO_result.xlsx
+++ b/smo/SMO_result.xlsx
@@ -458,10 +458,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>169702.5</v>
+        <v>120097.5</v>
       </c>
       <c r="D2" t="n">
-        <v>449.5</v>
+        <v>334.25</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>89715</v>
+        <v>58665</v>
       </c>
       <c r="D3" t="n">
-        <v>245</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4">
@@ -486,10 +486,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>57915</v>
+        <v>52357.5</v>
       </c>
       <c r="D4" t="n">
-        <v>208</v>
+        <v>204.5</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +500,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>69637.5</v>
+        <v>75120</v>
       </c>
       <c r="D5" t="n">
-        <v>210.75</v>
+        <v>206.75</v>
       </c>
     </row>
     <row r="6">
@@ -514,10 +514,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>91552.5</v>
+        <v>97462.5</v>
       </c>
       <c r="D6" t="n">
-        <v>210.75</v>
+        <v>206.5</v>
       </c>
     </row>
     <row r="7">
@@ -528,10 +528,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>115605</v>
+        <v>121770</v>
       </c>
       <c r="D7" t="n">
-        <v>210.25</v>
+        <v>206.5</v>
       </c>
     </row>
     <row r="8">
@@ -542,10 +542,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>140535</v>
+        <v>146527.5</v>
       </c>
       <c r="D8" t="n">
-        <v>210</v>
+        <v>206.5</v>
       </c>
     </row>
     <row r="9">
@@ -556,10 +556,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>165600</v>
+        <v>171307.5</v>
       </c>
       <c r="D9" t="n">
-        <v>210</v>
+        <v>206.5</v>
       </c>
     </row>
     <row r="10">
@@ -570,10 +570,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>191317.5</v>
+        <v>195930</v>
       </c>
       <c r="D10" t="n">
-        <v>210.25</v>
+        <v>206.5</v>
       </c>
     </row>
     <row r="11">
@@ -584,10 +584,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>216337.5</v>
+        <v>221047.5</v>
       </c>
       <c r="D11" t="n">
-        <v>210</v>
+        <v>206.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>